<commit_message>
feat: update login to main
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2b$12$wFl1nmNvCte7vgRhwCbDdu6fPdKma0goB.Tc6NmtNRjpnZfhCocoy</t>
+          <t>$2b$12$/Ktr48YHd6JHARagglOFgOD4FL9c5AkIce8NiPqfORjLemkEEoscS</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$/TWNahxIV8DV519MnXNZVeQL1U00v.rz/t2H9fkshNUbLNw/sGp4a</t>
+          <t>$2b$12$FCOwp2iPtCQ8YSTiF.L9P.d0VhWr8u7dBKKn42hpsJzNNiam8TfSO</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$2b$12$9MsmMfWc90q7f5kFVRTz9uYkV.80fCbd7J2gJtP.FHUs26tcu4a5u</t>
+          <t>$2b$12$gx7rkRUyzrgh8PDGSdhsFOvG2ncNrlxvzwmQEu4BCqR9IflkUbiIu</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$2b$12$bl5ghoz6u4M7.v1mnvI9zetFxAj8MQighsgwATDZNl2mW6fHP80Su</t>
+          <t>$2b$12$9xdq1qX.d9XK3ftfEHF0SuBy8JdIxKvr0b57jG5Tw2zA.PPL64hFm</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: change inicio page text
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2b$12$dnEm.7Uhx87Hlj5HIMIV4OtKrgEGbpyMzKxk1Fj.05svPQcCe3vB.</t>
+          <t>$2b$12$8/Iyol5kVAkJijBh9CVMhuEeMlNKHBKZAfa1GvcMtyFcD1BeuDIfy</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$iNQxdTs2Q2pdmYyYkvYrke2tRsiVaHHag8T/LIBqdp/kT5PldprVK</t>
+          <t>$2b$12$XFVj25dIinW2VVzVjzM5A.r9CHfH2opXiSyZw1wcP0naySiOJQeHO</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$2b$12$URKLT7SIDakWrHc7tUd2jOeDZdk/aIkTFKcBrJ6PG7TacpI/hQnFy</t>
+          <t>$2b$12$dNuOuP8WabQtRuuba8sadeOD9NsRpZBu3zHSpG5a/d04ZIOO3OLMa</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$2b$12$PERvjXXRGAkqcChk99atF.pmHy/l//vu9z5En1N5ovoW6qsE28UOG</t>
+          <t>$2b$12$B40wy1tIkOaJ7ZQDNAFG0O0j6gTFxowXbOi2ct.PUdtpqbH4Y/2Ui</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: passing user to home page
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2b$12$8/Iyol5kVAkJijBh9CVMhuEeMlNKHBKZAfa1GvcMtyFcD1BeuDIfy</t>
+          <t>$2b$12$5S12DDSfSY1d7mYVvJ8CBetURqyTzPtb3QBjH8hHSMwRRI.MnjP/2</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$XFVj25dIinW2VVzVjzM5A.r9CHfH2opXiSyZw1wcP0naySiOJQeHO</t>
+          <t>$2b$12$W/Ro6oHLXLgtZ2cL.xMslOjXkt2hPRGSiym88Kli9jtqJeLrrwsh6</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$2b$12$dNuOuP8WabQtRuuba8sadeOD9NsRpZBu3zHSpG5a/d04ZIOO3OLMa</t>
+          <t>$2b$12$9tmFMt9l/HZgYIZ5DWVM8.6CSSEU4zRgNBEIoe/o/H0oxY4pP5bcK</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$2b$12$B40wy1tIkOaJ7ZQDNAFG0O0j6gTFxowXbOi2ct.PUdtpqbH4Y/2Ui</t>
+          <t>$2b$12$x/1LHsLV2xKTfn915sPtb..DZIGsR9eEx7fftzyipz9XhH1E093oe</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add alunos on home page
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,43 +453,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2b$12$XndYNSVdTFlrR5iaiU/PHOhFMsTZFXlP9iIAGnIq4Uda6tbMulsfu</t>
+          <t>$2b$12$/or2YGXoZNVDkHa0iVcaGuZ7GK72fRUHAZCnpHcMF4IN2e8VwAXWC</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>diretor</t>
+          <t>aluno</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$sneYF8CKpmHdG6AvN2b0DOaZFbaahh7aKbrN2DSTP0BsFWfR6cWeC</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>professor</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>$2b$12$L67blNP4MK7hOflU2A5d5OtQnnEWGeI/ApYoHOYAefTJL.I11M.W2</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>aluno</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>$2b$12$IBcgFB.H8fSAhlfIPwEVAOvU44Gtl66aNIzzPKrbHZ9ywEBi4YdFq</t>
+          <t>$2b$12$L5aP6XHpk.FVIb0zVY5yR.8fttQPXKlcOy4U4u9qpwoTy32hsHW0W</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add users page to admin
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2b$12$/or2YGXoZNVDkHa0iVcaGuZ7GK72fRUHAZCnpHcMF4IN2e8VwAXWC</t>
+          <t>$2b$12$Gbe5kDlaOLxw31JaUunBhudpptax7CK8h2G.XJYJvHFNUwT6Rzmd2</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$L5aP6XHpk.FVIb0zVY5yR.8fttQPXKlcOy4U4u9qpwoTy32hsHW0W</t>
+          <t>$2b$12$69VZbrNp3/MXtilaHNl33ek3wTsohqttQRNJk1n2a31Vu6pTpvhjy</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: remove comments, unused imports, prints
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2b$12$Gbe5kDlaOLxw31JaUunBhudpptax7CK8h2G.XJYJvHFNUwT6Rzmd2</t>
+          <t>$2b$12$XXoSWoUxk3FaZ/QcTE4Ai.aSoo/csjhAQcT/RlAuYFQTDuyKwGDFa</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$69VZbrNp3/MXtilaHNl33ek3wTsohqttQRNJk1n2a31Vu6pTpvhjy</t>
+          <t>$2b$12$Cbtmniz9OFmXVPPrXx1syu9FNouKr4wb9zdMJdI2qQP.aqPp3z4YW</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: log out button
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2b$12$5KjtpoONTT8GfiKQNIw8oeAAzNPdm1Se4H3I7rpLh.A6mO7CNIr1m</t>
+          <t>$2b$12$4ekRDD1qm1OqI6uSGmffm.rZyJI2lIVM9XnMrUDBaYu4qYQJx.HD2</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$mG7NTK32l2yKYHcHOjofs./hp.9TVGwMAvm.q/xEUDI0.zCXg8fSy</t>
+          <t>$2b$12$6T.yFCTdqeTwtz9QX/TLRu5BOFAJ1ph2fE9annAvKSieD.U0wHbnW</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: exit button on login page
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2b$12$4ekRDD1qm1OqI6uSGmffm.rZyJI2lIVM9XnMrUDBaYu4qYQJx.HD2</t>
+          <t>$2b$12$MT5iMYj4wEOeXrfLN6E4vujkhN8EXI7sQUnIQWNycdGH7FcQzqcum</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$6T.yFCTdqeTwtz9QX/TLRu5BOFAJ1ph2fE9annAvKSieD.U0wHbnW</t>
+          <t>$2b$12$GwPM70p9B0N0F./Dz3YGauGR2KsumhBu9veD0vbJ2ZPSsQKVnKJP6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: update readme with video
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2b$12$MT5iMYj4wEOeXrfLN6E4vujkhN8EXI7sQUnIQWNycdGH7FcQzqcum</t>
+          <t>$2b$12$33Hg4/27rDv1L7idQFWrtu.47JsxM0EyrsGnll0VVLClWJ3FaCuKq</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$GwPM70p9B0N0F./Dz3YGauGR2KsumhBu9veD0vbJ2ZPSsQKVnKJP6</t>
+          <t>$2b$12$4sTvqqZ2JHwXsFTqdjpJLOAJOaWWLxSXzZs6aTLXjXZD2wPJOXBw6</t>
         </is>
       </c>
     </row>

</xml_diff>